<commit_message>
memory_layout 软件框图 SPI Flash datasheet
</commit_message>
<xml_diff>
--- a/Doc/design/软件框图.xlsx
+++ b/Doc/design/软件框图.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="795" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="目录" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>一、EnvMonitor系统功能划分简图</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -456,7 +456,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>二、系统启动</t>
+    <t>二、固件启动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三、</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -669,33 +673,28 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>278802</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>540219</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>119269</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPr id="2" name="图片 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -708,8 +707,155 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="57150" y="219075"/>
-          <a:ext cx="7765452" cy="10058400"/>
+          <a:off x="10270435" y="182217"/>
+          <a:ext cx="8789697" cy="7772400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>48815</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19050" y="200024"/>
+          <a:ext cx="11907440" cy="10715625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>96245</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>122885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>273653</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>161869</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="下箭头 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="3258711">
+          <a:off x="2699107" y="7854648"/>
+          <a:ext cx="210434" cy="4978008"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>36233</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="图片 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="219075" y="12001500"/>
+          <a:ext cx="7772400" cy="9980333"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1199,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N129"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130"/>
+    <sheetView tabSelected="1" topLeftCell="I22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R50" sqref="R50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1678,24 +1824,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A63"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+  <dimension ref="A1:A140"/>
+  <sheetViews>
+    <sheetView topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="2.875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="4" t="s">
+    <row r="70" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="4" t="s">
         <v>74</v>
       </c>
     </row>
+    <row r="140" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A140" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
USB to SPI Converter datasheet
</commit_message>
<xml_diff>
--- a/Doc/design/软件框图.xlsx
+++ b/Doc/design/软件框图.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="795" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="795" firstSheet="21" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="目录" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="UART Driver模块详细设计" sheetId="23" r:id="rId22"/>
     <sheet name="SystemDebug模块详细设计" sheetId="24" r:id="rId23"/>
     <sheet name="PinMuxCfg模块详细设计" sheetId="25" r:id="rId24"/>
-    <sheet name="BLE Service说 Driver模块详细设计" sheetId="26" r:id="rId25"/>
+    <sheet name="BLE Service Driver模块详细设计" sheetId="26" r:id="rId25"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -1131,13 +1131,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1755,25 +1755,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="25.5" x14ac:dyDescent="0.15">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
@@ -2398,8 +2398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4529,7 +4529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -4572,7 +4572,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="44" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>